<commit_message>
main.py df.to_csv missed index=False, sep=";"
</commit_message>
<xml_diff>
--- a/rivm_covid_19_data/rivm_covid_19_time_series/time_series_19-covid-Confirmed_province.xlsx
+++ b/rivm_covid_19_data/rivm_covid_19_time_series/time_series_19-covid-Confirmed_province.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>27-02-2020</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>08-03-2020</t>
+  </si>
+  <si>
+    <t>09-03-2020</t>
   </si>
   <si>
     <t>Provincienaam</t>
@@ -437,15 +440,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -480,10 +483,13 @@
       <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -518,10 +524,13 @@
       <c r="L2">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="M2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -556,10 +565,13 @@
       <c r="L3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="M3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -594,10 +606,13 @@
       <c r="L4">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="M4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -632,10 +647,13 @@
       <c r="L5">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="M5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -670,10 +688,13 @@
       <c r="L6">
         <v>93</v>
       </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="M6">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -708,10 +729,13 @@
       <c r="L7">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="M7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -746,10 +770,13 @@
       <c r="L8">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="M8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -784,10 +811,13 @@
       <c r="L9">
         <v>52</v>
       </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="M9">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -822,10 +852,13 @@
       <c r="L10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="M10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -859,6 +892,9 @@
       </c>
       <c r="L11">
         <v>34</v>
+      </c>
+      <c r="M11">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed main.py to make ints at "aantal"
</commit_message>
<xml_diff>
--- a/rivm_covid_19_data/rivm_covid_19_time_series/time_series_19-covid-Confirmed_province.xlsx
+++ b/rivm_covid_19_data/rivm_covid_19_time_series/time_series_19-covid-Confirmed_province.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>27-02-2020</t>
   </si>
@@ -52,6 +52,9 @@
     <t>09-03-2020</t>
   </si>
   <si>
+    <t>10-03-2020</t>
+  </si>
+  <si>
     <t>Provincienaam</t>
   </si>
   <si>
@@ -65,6 +68,9 @@
   </si>
   <si>
     <t>Gelderland</t>
+  </si>
+  <si>
+    <t>Groningen</t>
   </si>
   <si>
     <t>Limburg</t>
@@ -443,15 +449,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -489,10 +495,13 @@
       <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -530,10 +539,13 @@
       <c r="M2">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="N2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -571,10 +583,13 @@
       <c r="M3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="N3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -612,10 +627,13 @@
       <c r="M4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="N4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -653,292 +671,360 @@
       <c r="M5">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="N5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <v>10</v>
+      </c>
+      <c r="K7">
+        <v>11</v>
+      </c>
+      <c r="L7">
+        <v>16</v>
+      </c>
+      <c r="M7">
+        <v>23</v>
+      </c>
+      <c r="N7">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>8</v>
+      </c>
+      <c r="G8">
+        <v>12</v>
+      </c>
+      <c r="H8">
         <v>17</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>2</v>
-      </c>
-      <c r="J6">
+      <c r="I8">
+        <v>24</v>
+      </c>
+      <c r="J8">
+        <v>34</v>
+      </c>
+      <c r="K8">
+        <v>57</v>
+      </c>
+      <c r="L8">
+        <v>93</v>
+      </c>
+      <c r="M8">
+        <v>135</v>
+      </c>
+      <c r="N8">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="H9">
+        <v>7</v>
+      </c>
+      <c r="I9">
+        <v>9</v>
+      </c>
+      <c r="J9">
         <v>10</v>
       </c>
-      <c r="K6">
-        <v>11</v>
-      </c>
-      <c r="L6">
-        <v>16</v>
-      </c>
-      <c r="M6">
+      <c r="K9">
+        <v>17</v>
+      </c>
+      <c r="L9">
+        <v>22</v>
+      </c>
+      <c r="M9">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
-      <c r="E7">
-        <v>5</v>
-      </c>
-      <c r="F7">
-        <v>8</v>
-      </c>
-      <c r="G7">
+      <c r="N9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>4</v>
+      </c>
+      <c r="L10">
+        <v>9</v>
+      </c>
+      <c r="M10">
+        <v>10</v>
+      </c>
+      <c r="N10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="I11">
+        <v>23</v>
+      </c>
+      <c r="J11">
+        <v>33</v>
+      </c>
+      <c r="K11">
+        <v>47</v>
+      </c>
+      <c r="L11">
+        <v>52</v>
+      </c>
+      <c r="M11">
+        <v>52</v>
+      </c>
+      <c r="N11">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+      <c r="H13">
+        <v>7</v>
+      </c>
+      <c r="I13">
         <v>12</v>
       </c>
-      <c r="H7">
-        <v>17</v>
-      </c>
-      <c r="I7">
-        <v>24</v>
-      </c>
-      <c r="J7">
+      <c r="J13">
+        <v>23</v>
+      </c>
+      <c r="K13">
+        <v>29</v>
+      </c>
+      <c r="L13">
         <v>34</v>
       </c>
-      <c r="K7">
-        <v>57</v>
-      </c>
-      <c r="L7">
-        <v>93</v>
-      </c>
-      <c r="M7">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>3</v>
-      </c>
-      <c r="E8">
-        <v>3</v>
-      </c>
-      <c r="F8">
-        <v>3</v>
-      </c>
-      <c r="G8">
-        <v>3</v>
-      </c>
-      <c r="H8">
-        <v>7</v>
-      </c>
-      <c r="I8">
-        <v>9</v>
-      </c>
-      <c r="J8">
-        <v>10</v>
-      </c>
-      <c r="K8">
-        <v>17</v>
-      </c>
-      <c r="L8">
-        <v>22</v>
-      </c>
-      <c r="M8">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
-      <c r="K9">
-        <v>4</v>
-      </c>
-      <c r="L9">
-        <v>9</v>
-      </c>
-      <c r="M9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>3</v>
-      </c>
-      <c r="G10">
-        <v>3</v>
-      </c>
-      <c r="H10">
-        <v>3</v>
-      </c>
-      <c r="I10">
-        <v>23</v>
-      </c>
-      <c r="J10">
-        <v>33</v>
-      </c>
-      <c r="K10">
+      <c r="M13">
+        <v>37</v>
+      </c>
+      <c r="N13">
         <v>47</v>
-      </c>
-      <c r="L10">
-        <v>52</v>
-      </c>
-      <c r="M10">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
-      <c r="L11">
-        <v>1</v>
-      </c>
-      <c r="M11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>2</v>
-      </c>
-      <c r="F12">
-        <v>3</v>
-      </c>
-      <c r="G12">
-        <v>3</v>
-      </c>
-      <c r="H12">
-        <v>7</v>
-      </c>
-      <c r="I12">
-        <v>12</v>
-      </c>
-      <c r="J12">
-        <v>23</v>
-      </c>
-      <c r="K12">
-        <v>29</v>
-      </c>
-      <c r="L12">
-        <v>34</v>
-      </c>
-      <c r="M12">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added provinciecode to df.
</commit_message>
<xml_diff>
--- a/rivm_covid_19_data/rivm_covid_19_time_series/time_series_19-covid-Confirmed_province.xlsx
+++ b/rivm_covid_19_data/rivm_covid_19_time_series/time_series_19-covid-Confirmed_province.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>27-02-2020</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>Provincienaam</t>
+  </si>
+  <si>
+    <t>Provinciecode</t>
   </si>
   <si>
     <t>Drenthe</t>
@@ -449,62 +452,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:15">
       <c r="A2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="B2" s="1">
+        <v>22</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -513,19 +519,19 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <v>2</v>
       </c>
       <c r="I2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J2">
         <v>3</v>
@@ -534,21 +540,24 @@
         <v>3</v>
       </c>
       <c r="L2">
+        <v>3</v>
+      </c>
+      <c r="M2">
         <v>8</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>10</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:15">
       <c r="A3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="B3" s="1">
+        <v>24</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -569,10 +578,10 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K3">
         <v>2</v>
@@ -586,365 +595,392 @@
       <c r="N3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="O3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1">
+        <v>21</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1">
+        <v>25</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <v>10</v>
+      </c>
+      <c r="L5">
+        <v>13</v>
+      </c>
+      <c r="M5">
+        <v>26</v>
+      </c>
+      <c r="N5">
+        <v>27</v>
+      </c>
+      <c r="O5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1">
+        <v>31</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <v>10</v>
+      </c>
+      <c r="L7">
+        <v>11</v>
+      </c>
+      <c r="M7">
         <v>16</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="1" t="s">
+      <c r="N7">
+        <v>23</v>
+      </c>
+      <c r="O7">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="1">
+        <v>30</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+      <c r="G8">
+        <v>8</v>
+      </c>
+      <c r="H8">
+        <v>12</v>
+      </c>
+      <c r="I8">
         <v>17</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>2</v>
-      </c>
-      <c r="J5">
+      <c r="J8">
+        <v>24</v>
+      </c>
+      <c r="K8">
+        <v>34</v>
+      </c>
+      <c r="L8">
+        <v>57</v>
+      </c>
+      <c r="M8">
+        <v>93</v>
+      </c>
+      <c r="N8">
+        <v>135</v>
+      </c>
+      <c r="O8">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1">
+        <v>27</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="I9">
+        <v>7</v>
+      </c>
+      <c r="J9">
+        <v>9</v>
+      </c>
+      <c r="K9">
         <v>10</v>
       </c>
-      <c r="K5">
-        <v>13</v>
-      </c>
-      <c r="L5">
-        <v>26</v>
-      </c>
-      <c r="M5">
-        <v>27</v>
-      </c>
-      <c r="N5">
+      <c r="L9">
+        <v>17</v>
+      </c>
+      <c r="M9">
+        <v>22</v>
+      </c>
+      <c r="N9">
+        <v>23</v>
+      </c>
+      <c r="O9">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="A7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>2</v>
-      </c>
-      <c r="J7">
-        <v>10</v>
-      </c>
-      <c r="K7">
-        <v>11</v>
-      </c>
-      <c r="L7">
-        <v>16</v>
-      </c>
-      <c r="M7">
+    <row r="10" spans="1:15">
+      <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N7">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>3</v>
-      </c>
-      <c r="E8">
-        <v>5</v>
-      </c>
-      <c r="F8">
-        <v>8</v>
-      </c>
-      <c r="G8">
-        <v>12</v>
-      </c>
-      <c r="H8">
-        <v>17</v>
-      </c>
-      <c r="I8">
-        <v>24</v>
-      </c>
-      <c r="J8">
-        <v>34</v>
-      </c>
-      <c r="K8">
-        <v>57</v>
-      </c>
-      <c r="L8">
-        <v>93</v>
-      </c>
-      <c r="M8">
-        <v>135</v>
-      </c>
-      <c r="N8">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
-      <c r="A9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>3</v>
-      </c>
-      <c r="E9">
-        <v>3</v>
-      </c>
-      <c r="F9">
-        <v>3</v>
-      </c>
-      <c r="G9">
-        <v>3</v>
-      </c>
-      <c r="H9">
-        <v>7</v>
-      </c>
-      <c r="I9">
+      <c r="B10" s="1">
+        <v>23</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>4</v>
+      </c>
+      <c r="M10">
         <v>9</v>
-      </c>
-      <c r="J9">
-        <v>10</v>
-      </c>
-      <c r="K9">
-        <v>17</v>
-      </c>
-      <c r="L9">
-        <v>22</v>
-      </c>
-      <c r="M9">
-        <v>23</v>
-      </c>
-      <c r="N9">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="A10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="K10">
-        <v>4</v>
-      </c>
-      <c r="L10">
-        <v>9</v>
-      </c>
-      <c r="M10">
-        <v>10</v>
       </c>
       <c r="N10">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:14">
+      <c r="O10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="1">
+        <v>26</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="I11">
+        <v>3</v>
+      </c>
+      <c r="J11">
         <v>23</v>
       </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>3</v>
-      </c>
-      <c r="G11">
-        <v>3</v>
-      </c>
-      <c r="H11">
-        <v>3</v>
-      </c>
-      <c r="I11">
-        <v>23</v>
-      </c>
-      <c r="J11">
+      <c r="K11">
         <v>33</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>47</v>
-      </c>
-      <c r="L11">
-        <v>52</v>
       </c>
       <c r="M11">
         <v>52</v>
       </c>
       <c r="N11">
+        <v>52</v>
+      </c>
+      <c r="O11">
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:15">
       <c r="A12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
+        <v>25</v>
+      </c>
+      <c r="B12" s="1">
+        <v>29</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -971,7 +1007,7 @@
         <v>0</v>
       </c>
       <c r="K12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L12">
         <v>1</v>
@@ -980,50 +1016,56 @@
         <v>1</v>
       </c>
       <c r="N12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="B13" s="1">
+        <v>28</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G13">
         <v>3</v>
       </c>
       <c r="H13">
+        <v>3</v>
+      </c>
+      <c r="I13">
         <v>7</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>12</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>23</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>29</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>34</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>37</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed index order provincie
</commit_message>
<xml_diff>
--- a/rivm_covid_19_data/rivm_covid_19_time_series/time_series_19-covid-Confirmed_province.xlsx
+++ b/rivm_covid_19_data/rivm_covid_19_time_series/time_series_19-covid-Confirmed_province.xlsx
@@ -55,10 +55,10 @@
     <t>10-03-2020</t>
   </si>
   <si>
+    <t>Provinciecode</t>
+  </si>
+  <si>
     <t>Provincienaam</t>
-  </si>
-  <si>
-    <t>Provinciecode</t>
   </si>
   <si>
     <t>Drenthe</t>
@@ -506,11 +506,11 @@
       </c>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="1">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B2" s="1">
-        <v>22</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -553,12 +553,12 @@
       </c>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="1">
+        <v>24</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="1">
-        <v>24</v>
-      </c>
       <c r="C3">
         <v>0</v>
       </c>
@@ -600,12 +600,12 @@
       </c>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="1">
+        <v>21</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="1">
-        <v>21</v>
-      </c>
       <c r="C4">
         <v>0</v>
       </c>
@@ -647,11 +647,11 @@
       </c>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="1">
+        <v>25</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B5" s="1">
-        <v>25</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -694,58 +694,58 @@
       </c>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="1">
+        <v>20</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="1">
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="1">
+        <v>31</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
-      <c r="A7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="1">
-        <v>31</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -788,11 +788,11 @@
       </c>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="1">
+        <v>30</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B8" s="1">
-        <v>30</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -835,11 +835,11 @@
       </c>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="1">
+        <v>27</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="B9" s="1">
-        <v>27</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -882,10 +882,10 @@
       </c>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="1">
         <v>23</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C10">
@@ -929,11 +929,11 @@
       </c>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="1">
+        <v>26</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="B11" s="1">
-        <v>26</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -976,12 +976,12 @@
       </c>
     </row>
     <row r="12" spans="1:15">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="1">
+        <v>29</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="1">
-        <v>29</v>
-      </c>
       <c r="C12">
         <v>0</v>
       </c>
@@ -1023,11 +1023,11 @@
       </c>
     </row>
     <row r="13" spans="1:15">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="1">
+        <v>28</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B13" s="1">
-        <v>28</v>
       </c>
       <c r="C13">
         <v>0</v>

</xml_diff>